<commit_message>
excel report hls aggiornato
</commit_message>
<xml_diff>
--- a/reports/hls/report-hls-solutions.xlsx
+++ b/reports/hls/report-hls-solutions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Disco D\universita\magistrale\sintesi-ad-alto-livello-di-sistemi-digitali\progetti\progetto1\reports\hls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2171D712-A15F-4E4D-9FF8-70A9568D66F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3F95B8-7BCB-458A-8041-6FA26E65A96F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{478786F9-0C08-4B95-A9F2-D12EA5517A72}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="66">
   <si>
     <t>Unoptimized</t>
   </si>
@@ -234,6 +234,9 @@
   </si>
   <si>
     <t>3~12</t>
+  </si>
+  <si>
+    <t>Bitwidth Optimization</t>
   </si>
 </sst>
 </file>
@@ -467,22 +470,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -494,16 +527,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -515,37 +548,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -689,13 +692,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$B$8:$B$28</c15:sqref>
+                    <c15:sqref>Data!$B$8:$B$29</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$28)</c:f>
+              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$29)</c:f>
               <c:strCache>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>Unoptimized</c:v>
                 </c:pt>
@@ -748,6 +751,9 @@
                   <c:v>Loop Pipelining</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>Bitwidth Optimization</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>AXI</c:v>
                 </c:pt>
               </c:strCache>
@@ -758,14 +764,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$D$8:$D$28</c15:sqref>
+                    <c15:sqref>Data!$D$8:$D$29</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$D$8:$D$10,Data!$D$12,Data!$D$14:$D$16,Data!$D$18:$D$28)</c:f>
+              <c:f>(Data!$D$8:$D$10,Data!$D$12,Data!$D$14:$D$16,Data!$D$18:$D$29)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -818,6 +824,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -874,13 +883,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$B$8:$B$28</c15:sqref>
+                    <c15:sqref>Data!$B$8:$B$29</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$28)</c:f>
+              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$29)</c:f>
               <c:strCache>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>Unoptimized</c:v>
                 </c:pt>
@@ -933,6 +942,9 @@
                   <c:v>Loop Pipelining</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>Bitwidth Optimization</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>AXI</c:v>
                 </c:pt>
               </c:strCache>
@@ -943,14 +955,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$E$8:$E$28</c15:sqref>
+                    <c15:sqref>Data!$E$8:$E$29</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$E$8:$E$10,Data!$E$12,Data!$E$14:$E$16,Data!$E$18:$E$28)</c:f>
+              <c:f>(Data!$E$8:$E$10,Data!$E$12,Data!$E$14:$E$16,Data!$E$18:$E$29)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>4</c:v>
                 </c:pt>
@@ -1003,6 +1015,9 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
@@ -1059,13 +1074,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$B$8:$B$28</c15:sqref>
+                    <c15:sqref>Data!$B$8:$B$29</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$28)</c:f>
+              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$29)</c:f>
               <c:strCache>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>Unoptimized</c:v>
                 </c:pt>
@@ -1118,6 +1133,9 @@
                   <c:v>Loop Pipelining</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>Bitwidth Optimization</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>AXI</c:v>
                 </c:pt>
               </c:strCache>
@@ -1128,14 +1146,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$F$8:$F$28</c15:sqref>
+                    <c15:sqref>Data!$F$8:$F$29</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$F$8:$F$10,Data!$F$12,Data!$F$14:$F$16,Data!$F$18:$F$28)</c:f>
+              <c:f>(Data!$F$8:$F$10,Data!$F$12,Data!$F$14:$F$16,Data!$F$18:$F$29)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>287</c:v>
                 </c:pt>
@@ -1188,6 +1206,9 @@
                   <c:v>710</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>767</c:v>
                 </c:pt>
               </c:numCache>
@@ -1242,13 +1263,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$B$8:$B$28</c15:sqref>
+                    <c15:sqref>Data!$B$8:$B$29</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$28)</c:f>
+              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$29)</c:f>
               <c:strCache>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>Unoptimized</c:v>
                 </c:pt>
@@ -1301,6 +1322,9 @@
                   <c:v>Loop Pipelining</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>Bitwidth Optimization</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>AXI</c:v>
                 </c:pt>
               </c:strCache>
@@ -1311,14 +1335,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$G$8:$G$28</c15:sqref>
+                    <c15:sqref>Data!$G$8:$G$29</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$G$8:$G$10,Data!$G$12,Data!$G$14:$G$16,Data!$G$18:$G$28)</c:f>
+              <c:f>(Data!$G$8:$G$10,Data!$G$12,Data!$G$14:$G$16,Data!$G$18:$G$29)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>233</c:v>
                 </c:pt>
@@ -1371,6 +1395,9 @@
                   <c:v>621</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>583</c:v>
                 </c:pt>
               </c:numCache>
@@ -1435,7 +1462,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1773,13 +1800,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$B$8:$B$27</c15:sqref>
+                    <c15:sqref>Data!$B$8:$B$28</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$27)</c:f>
+              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$28)</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>Unoptimized</c:v>
                 </c:pt>
@@ -1830,6 +1857,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>Loop Pipelining</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Bitwidth Optimization</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1839,14 +1869,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$K$8:$K$27</c15:sqref>
+                    <c15:sqref>Data!$K$8:$K$28</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$K$8:$K$10,Data!$K$12,Data!$K$14:$K$16,Data!$K$18:$K$27)</c:f>
+              <c:f>(Data!$K$8:$K$10,Data!$K$12,Data!$K$14:$K$16,Data!$K$18:$K$28)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>23</c:v>
                 </c:pt>
@@ -1897,6 +1927,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1952,13 +1985,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$B$8:$B$27</c15:sqref>
+                    <c15:sqref>Data!$B$8:$B$28</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$27)</c:f>
+              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$28)</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>Unoptimized</c:v>
                 </c:pt>
@@ -2009,6 +2042,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>Loop Pipelining</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Bitwidth Optimization</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2018,14 +2054,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$L$8:$L$27</c15:sqref>
+                    <c15:sqref>Data!$L$8:$L$28</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$L$8:$L$10,Data!$L$12,Data!$L$14:$L$16,Data!$L$18:$L$27)</c:f>
+              <c:f>(Data!$L$8:$L$10,Data!$L$12,Data!$L$14:$L$16,Data!$L$18:$L$28)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>45</c:v>
                 </c:pt>
@@ -2076,6 +2112,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2139,7 +2178,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -2470,13 +2509,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$B$8:$B$27</c15:sqref>
+                    <c15:sqref>Data!$B$8:$B$28</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$27)</c:f>
+              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$28)</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>Unoptimized</c:v>
                 </c:pt>
@@ -2527,6 +2566,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>Loop Pipelining</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Bitwidth Optimization</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2536,14 +2578,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$M$8:$M$27</c15:sqref>
+                    <c15:sqref>Data!$M$8:$M$28</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$M$8:$M$10,Data!$M$12,Data!$M$14:$M$16,Data!$M$18:$M$27)</c:f>
+              <c:f>(Data!$M$8:$M$10,Data!$M$12,Data!$M$14:$M$16,Data!$M$18:$M$28)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>23</c:v>
                 </c:pt>
@@ -2594,6 +2636,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2649,13 +2694,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$B$8:$B$27</c15:sqref>
+                    <c15:sqref>Data!$B$8:$B$28</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$27)</c:f>
+              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$28)</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>Unoptimized</c:v>
                 </c:pt>
@@ -2706,6 +2751,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>Loop Pipelining</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Bitwidth Optimization</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2715,14 +2763,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$N$8:$N$27</c15:sqref>
+                    <c15:sqref>Data!$N$8:$N$28</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$N$8:$N$10,Data!$N$12,Data!$N$14:$N$16,Data!$N$18:$N$27)</c:f>
+              <c:f>(Data!$N$8:$N$10,Data!$N$12,Data!$N$14:$N$16,Data!$N$18:$N$28)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>45</c:v>
                 </c:pt>
@@ -2773,6 +2821,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2836,7 +2887,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -3142,13 +3193,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$B$8:$B$27</c15:sqref>
+                    <c15:sqref>Data!$B$8:$B$28</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$27)</c:f>
+              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$28)</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>Unoptimized</c:v>
                 </c:pt>
@@ -3199,6 +3250,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>Loop Pipelining</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Bitwidth Optimization</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3208,14 +3262,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$U$8:$U$27</c15:sqref>
+                    <c15:sqref>Data!$U$8:$U$28</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$U$8:$U$10,Data!$U$12,Data!$U$14:$U$16,Data!$U$18:$U$27)</c:f>
+              <c:f>(Data!$U$8:$U$10,Data!$U$12,Data!$U$14:$U$16,Data!$U$18:$U$28)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>11</c:v>
                 </c:pt>
@@ -3266,6 +3320,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3329,7 +3386,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -3660,13 +3717,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$B$8:$B$27</c15:sqref>
+                    <c15:sqref>Data!$B$8:$B$28</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$27)</c:f>
+              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$28)</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>Unoptimized</c:v>
                 </c:pt>
@@ -3717,6 +3774,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>Loop Pipelining</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Bitwidth Optimization</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3726,14 +3786,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$X$8:$X$27</c15:sqref>
+                    <c15:sqref>Data!$X$8:$X$28</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$X$8:$X$10,Data!$X$12,Data!$X$14:$X$16,Data!$X$18:$X$27)</c:f>
+              <c:f>(Data!$X$8:$X$10,Data!$X$12,Data!$X$14:$X$16,Data!$X$18:$X$28)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>43</c:v>
                 </c:pt>
@@ -3784,6 +3844,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3839,13 +3902,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$B$8:$B$27</c15:sqref>
+                    <c15:sqref>Data!$B$8:$B$28</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$27)</c:f>
+              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$28)</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>Unoptimized</c:v>
                 </c:pt>
@@ -3896,6 +3959,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>Loop Pipelining</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Bitwidth Optimization</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3905,14 +3971,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$Y$8:$Y$27</c15:sqref>
+                    <c15:sqref>Data!$Y$8:$Y$28</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$Y$8:$Y$10,Data!$Y$12,Data!$Y$14:$Y$16,Data!$Y$18:$Y$27)</c:f>
+              <c:f>(Data!$Y$8:$Y$10,Data!$Y$12,Data!$Y$14:$Y$16,Data!$Y$18:$Y$28)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>43</c:v>
                 </c:pt>
@@ -3963,6 +4029,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4018,13 +4087,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$B$8:$B$27</c15:sqref>
+                    <c15:sqref>Data!$B$8:$B$28</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$27)</c:f>
+              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$28)</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>Unoptimized</c:v>
                 </c:pt>
@@ -4075,6 +4144,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>Loop Pipelining</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Bitwidth Optimization</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4084,14 +4156,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$Z$8:$Z$27</c15:sqref>
+                    <c15:sqref>Data!$Z$8:$Z$28</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$Z$8:$Z$10,Data!$Z$12,Data!$Z$14:$Z$16,Data!$Z$18:$Z$27)</c:f>
+              <c:f>(Data!$Z$8:$Z$10,Data!$Z$12,Data!$Z$14:$Z$16,Data!$Z$18:$Z$28)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>44</c:v>
                 </c:pt>
@@ -4142,6 +4214,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4205,7 +4280,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -4536,13 +4611,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$B$8:$B$27</c15:sqref>
+                    <c15:sqref>Data!$B$8:$B$28</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$27)</c:f>
+              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$28)</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>Unoptimized</c:v>
                 </c:pt>
@@ -4593,6 +4668,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>Loop Pipelining</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Bitwidth Optimization</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4602,14 +4680,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$AA$8:$AA$27</c15:sqref>
+                    <c15:sqref>Data!$AA$8:$AA$28</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$AA$8:$AA$10,Data!$AA$12,Data!$AA$14:$AA$16,Data!$AA$18:$AA$27)</c:f>
+              <c:f>(Data!$AA$8:$AA$10,Data!$AA$12,Data!$AA$14:$AA$16,Data!$AA$18:$AA$28)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>43</c:v>
                 </c:pt>
@@ -4660,6 +4738,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4715,13 +4796,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$B$8:$B$27</c15:sqref>
+                    <c15:sqref>Data!$B$8:$B$28</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$27)</c:f>
+              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$28)</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>Unoptimized</c:v>
                 </c:pt>
@@ -4772,6 +4853,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>Loop Pipelining</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Bitwidth Optimization</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4781,14 +4865,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$AB$8:$AB$27</c15:sqref>
+                    <c15:sqref>Data!$AB$8:$AB$28</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$AB$8:$AB$10,Data!$AB$12,Data!$AB$14:$AB$16,Data!$AB$18:$AB$27)</c:f>
+              <c:f>(Data!$AB$8:$AB$10,Data!$AB$12,Data!$AB$14:$AB$16,Data!$AB$18:$AB$28)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>43</c:v>
                 </c:pt>
@@ -4839,6 +4923,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4894,13 +4981,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$B$8:$B$27</c15:sqref>
+                    <c15:sqref>Data!$B$8:$B$28</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$27)</c:f>
+              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$28)</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>Unoptimized</c:v>
                 </c:pt>
@@ -4951,6 +5038,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>Loop Pipelining</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Bitwidth Optimization</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4960,14 +5050,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$AC$8:$AC$27</c15:sqref>
+                    <c15:sqref>Data!$AC$8:$AC$28</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$AC$8:$AC$10,Data!$AC$12,Data!$AC$14:$AC$16,Data!$AC$18:$AC$27)</c:f>
+              <c:f>(Data!$AC$8:$AC$10,Data!$AC$12,Data!$AC$14:$AC$16,Data!$AC$18:$AC$28)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>44</c:v>
                 </c:pt>
@@ -5018,6 +5108,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5412,13 +5505,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$B$8:$B$28</c15:sqref>
+                    <c15:sqref>Data!$B$8:$B$29</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$28)</c:f>
+              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$29)</c:f>
               <c:strCache>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>Unoptimized</c:v>
                 </c:pt>
@@ -5471,6 +5564,9 @@
                   <c:v>Loop Pipelining</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>Bitwidth Optimization</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>AXI</c:v>
                 </c:pt>
               </c:strCache>
@@ -5481,14 +5577,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$AF$8:$AF$28</c15:sqref>
+                    <c15:sqref>Data!$AF$8:$AF$29</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$AF$8:$AF$10,Data!$AF$12,Data!$AF$14:$AF$16,Data!$AF$18:$AF$28)</c:f>
+              <c:f>(Data!$AF$8:$AF$10,Data!$AF$12,Data!$AF$14:$AF$16,Data!$AF$18:$AF$29)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>81</c:v>
                 </c:pt>
@@ -5541,6 +5637,9 @@
                   <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>231</c:v>
                 </c:pt>
               </c:numCache>
@@ -5597,13 +5696,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$B$8:$B$28</c15:sqref>
+                    <c15:sqref>Data!$B$8:$B$29</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$28)</c:f>
+              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$29)</c:f>
               <c:strCache>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>Unoptimized</c:v>
                 </c:pt>
@@ -5656,6 +5755,9 @@
                   <c:v>Loop Pipelining</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>Bitwidth Optimization</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>AXI</c:v>
                 </c:pt>
               </c:strCache>
@@ -5666,14 +5768,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$AG$8:$AG$28</c15:sqref>
+                    <c15:sqref>Data!$AG$8:$AG$29</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$AG$8:$AG$10,Data!$AG$12,Data!$AG$14:$AG$16,Data!$AG$18:$AG$28)</c:f>
+              <c:f>(Data!$AG$8:$AG$10,Data!$AG$12,Data!$AG$14:$AG$16,Data!$AG$18:$AG$29)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>275</c:v>
                 </c:pt>
@@ -5726,6 +5828,9 @@
                   <c:v>311</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>739</c:v>
                 </c:pt>
               </c:numCache>
@@ -5782,13 +5887,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$B$8:$B$28</c15:sqref>
+                    <c15:sqref>Data!$B$8:$B$29</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$28)</c:f>
+              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$29)</c:f>
               <c:strCache>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>Unoptimized</c:v>
                 </c:pt>
@@ -5841,6 +5946,9 @@
                   <c:v>Loop Pipelining</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>Bitwidth Optimization</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>AXI</c:v>
                 </c:pt>
               </c:strCache>
@@ -5851,14 +5959,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$AH$8:$AH$28</c15:sqref>
+                    <c15:sqref>Data!$AH$8:$AH$29</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$AH$8:$AH$10,Data!$AH$12,Data!$AH$14:$AH$16,Data!$AH$18:$AH$28)</c:f>
+              <c:f>(Data!$AH$8:$AH$10,Data!$AH$12,Data!$AH$14:$AH$16,Data!$AH$18:$AH$29)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>160</c:v>
                 </c:pt>
@@ -5911,6 +6019,9 @@
                   <c:v>455</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>699</c:v>
                 </c:pt>
               </c:numCache>
@@ -5965,13 +6076,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$B$8:$B$28</c15:sqref>
+                    <c15:sqref>Data!$B$8:$B$29</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$28)</c:f>
+              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$29)</c:f>
               <c:strCache>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>Unoptimized</c:v>
                 </c:pt>
@@ -6024,6 +6135,9 @@
                   <c:v>Loop Pipelining</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>Bitwidth Optimization</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>AXI</c:v>
                 </c:pt>
               </c:strCache>
@@ -6034,14 +6148,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$AI$8:$AI$28</c15:sqref>
+                    <c15:sqref>Data!$AI$8:$AI$29</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$AI$8:$AI$10,Data!$AI$12,Data!$AI$14:$AI$16,Data!$AI$18:$AI$28)</c:f>
+              <c:f>(Data!$AI$8:$AI$10,Data!$AI$12,Data!$AI$14:$AI$16,Data!$AI$18:$AI$29)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -6094,6 +6208,9 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -6148,13 +6265,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$B$8:$B$28</c15:sqref>
+                    <c15:sqref>Data!$B$8:$B$29</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$28)</c:f>
+              <c:f>(Data!$B$8:$B$10,Data!$B$12,Data!$B$14:$B$16,Data!$B$18:$B$29)</c:f>
               <c:strCache>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>Unoptimized</c:v>
                 </c:pt>
@@ -6207,6 +6324,9 @@
                   <c:v>Loop Pipelining</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>Bitwidth Optimization</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>AXI</c:v>
                 </c:pt>
               </c:strCache>
@@ -6217,14 +6337,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Data!$AJ$8:$AJ$28</c15:sqref>
+                    <c15:sqref>Data!$AJ$8:$AJ$29</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Data!$AJ$8:$AJ$10,Data!$AJ$12,Data!$AJ$14:$AJ$16,Data!$AJ$18:$AJ$28)</c:f>
+              <c:f>(Data!$AJ$8:$AJ$10,Data!$AJ$12,Data!$AJ$14:$AJ$16,Data!$AJ$18:$AJ$29)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -6277,6 +6397,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -6341,7 +6464,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -10497,8 +10620,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>593912</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
@@ -10533,8 +10656,8 @@
       <xdr:rowOff>168088</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>11205</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>188962</xdr:rowOff>
     </xdr:to>
@@ -10563,16 +10686,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>179295</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>324970</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>336177</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>22412</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10599,14 +10722,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>313765</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>369794</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>13446</xdr:rowOff>
     </xdr:to>
@@ -10646,8 +10769,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>600074</xdr:colOff>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>17144</xdr:rowOff>
     </xdr:to>
@@ -10676,16 +10799,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>612775</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>10584</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>603249</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>17144</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>607218</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>27728</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10725,8 +10848,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>17144</xdr:rowOff>
     </xdr:to>
@@ -11073,10 +11196,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C32F8C0C-32ED-409A-A129-79038668F278}">
-  <dimension ref="B2:AP28"/>
+  <dimension ref="B2:AP29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AG35" sqref="AG35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11104,242 +11227,242 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:42" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="18"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="35"/>
       <c r="V2" s="7"/>
-      <c r="X2" s="18" t="s">
+      <c r="X2" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="18"/>
-      <c r="Z2" s="18"/>
-      <c r="AA2" s="18"/>
-      <c r="AB2" s="18"/>
-      <c r="AC2" s="18"/>
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="35"/>
+      <c r="AA2" s="35"/>
+      <c r="AB2" s="35"/>
+      <c r="AC2" s="35"/>
       <c r="AD2" s="7"/>
-      <c r="AF2" s="18" t="s">
+      <c r="AF2" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="AG2" s="18"/>
-      <c r="AH2" s="18"/>
-      <c r="AI2" s="18"/>
-      <c r="AJ2" s="18"/>
-      <c r="AK2" s="18"/>
-      <c r="AL2" s="18"/>
-      <c r="AM2" s="18"/>
-      <c r="AN2" s="18"/>
+      <c r="AG2" s="35"/>
+      <c r="AH2" s="35"/>
+      <c r="AI2" s="35"/>
+      <c r="AJ2" s="35"/>
+      <c r="AK2" s="35"/>
+      <c r="AL2" s="35"/>
+      <c r="AM2" s="35"/>
+      <c r="AN2" s="35"/>
     </row>
     <row r="3" spans="2:42" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="24" t="s">
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="I3" s="25"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="24" t="s">
+      <c r="I3" s="21"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37"/>
-      <c r="U3" s="38"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="27"/>
+      <c r="R3" s="27"/>
+      <c r="S3" s="27"/>
+      <c r="T3" s="27"/>
+      <c r="U3" s="28"/>
       <c r="V3" s="7"/>
-      <c r="X3" s="24" t="s">
+      <c r="X3" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Y3" s="25"/>
-      <c r="Z3" s="33"/>
-      <c r="AA3" s="24" t="s">
+      <c r="Y3" s="21"/>
+      <c r="Z3" s="22"/>
+      <c r="AA3" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AB3" s="25"/>
-      <c r="AC3" s="33"/>
-      <c r="AF3" s="24" t="s">
+      <c r="AB3" s="21"/>
+      <c r="AC3" s="22"/>
+      <c r="AF3" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="AG3" s="25"/>
-      <c r="AH3" s="25"/>
-      <c r="AI3" s="25"/>
-      <c r="AJ3" s="25"/>
-      <c r="AK3" s="33"/>
-      <c r="AL3" s="24" t="s">
+      <c r="AG3" s="21"/>
+      <c r="AH3" s="21"/>
+      <c r="AI3" s="21"/>
+      <c r="AJ3" s="21"/>
+      <c r="AK3" s="22"/>
+      <c r="AL3" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="AM3" s="25"/>
-      <c r="AN3" s="25"/>
+      <c r="AM3" s="21"/>
+      <c r="AN3" s="21"/>
       <c r="AO3" s="4"/>
     </row>
     <row r="4" spans="2:42" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="39" t="s">
+      <c r="G4" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="39" t="s">
+      <c r="J4" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="29" t="s">
+      <c r="K4" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="39"/>
-      <c r="M4" s="29" t="s">
+      <c r="L4" s="16"/>
+      <c r="M4" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="N4" s="30"/>
-      <c r="O4" s="19" t="s">
+      <c r="N4" s="32"/>
+      <c r="O4" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="20"/>
-      <c r="S4" s="20"/>
-      <c r="T4" s="20"/>
-      <c r="U4" s="21"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="30"/>
+      <c r="U4" s="31"/>
       <c r="V4" s="7"/>
-      <c r="X4" s="22" t="s">
+      <c r="X4" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="Y4" s="22" t="s">
+      <c r="Y4" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="Z4" s="22" t="s">
+      <c r="Z4" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="AA4" s="22" t="s">
+      <c r="AA4" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AB4" s="22" t="s">
+      <c r="AB4" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="AC4" s="22" t="s">
+      <c r="AC4" s="13" t="s">
         <v>30</v>
       </c>
       <c r="AD4" s="7"/>
-      <c r="AF4" s="22" t="s">
+      <c r="AF4" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="AG4" s="22" t="s">
+      <c r="AG4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="AH4" s="22" t="s">
+      <c r="AH4" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="AI4" s="22" t="s">
+      <c r="AI4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="AJ4" s="22" t="s">
+      <c r="AJ4" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="AK4" s="22" t="s">
+      <c r="AK4" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="AL4" s="22" t="s">
+      <c r="AL4" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="AM4" s="26" t="s">
+      <c r="AM4" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="AN4" s="26" t="s">
+      <c r="AN4" s="36" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="5" spans="2:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="22" t="s">
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="P5" s="34" t="s">
+      <c r="P5" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="Q5" s="35"/>
-      <c r="R5" s="13" t="s">
+      <c r="Q5" s="24"/>
+      <c r="R5" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="S5" s="34" t="s">
+      <c r="S5" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="T5" s="35"/>
-      <c r="U5" s="13" t="s">
+      <c r="T5" s="24"/>
+      <c r="U5" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="X5" s="16"/>
-      <c r="Y5" s="16"/>
-      <c r="Z5" s="16"/>
-      <c r="AA5" s="16"/>
-      <c r="AB5" s="16"/>
-      <c r="AC5" s="16"/>
-      <c r="AF5" s="16"/>
-      <c r="AG5" s="16"/>
-      <c r="AH5" s="16"/>
-      <c r="AI5" s="16"/>
-      <c r="AJ5" s="16"/>
-      <c r="AK5" s="16"/>
-      <c r="AL5" s="16"/>
-      <c r="AM5" s="27"/>
-      <c r="AN5" s="27"/>
+      <c r="X5" s="14"/>
+      <c r="Y5" s="14"/>
+      <c r="Z5" s="14"/>
+      <c r="AA5" s="14"/>
+      <c r="AB5" s="14"/>
+      <c r="AC5" s="14"/>
+      <c r="AF5" s="14"/>
+      <c r="AG5" s="14"/>
+      <c r="AH5" s="14"/>
+      <c r="AI5" s="14"/>
+      <c r="AJ5" s="14"/>
+      <c r="AK5" s="14"/>
+      <c r="AL5" s="14"/>
+      <c r="AM5" s="37"/>
+      <c r="AN5" s="37"/>
     </row>
     <row r="6" spans="2:42" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="32"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="17"/>
       <c r="K6" s="10" t="s">
         <v>29</v>
       </c>
@@ -11352,38 +11475,38 @@
       <c r="N6" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="O6" s="23"/>
+      <c r="O6" s="15"/>
       <c r="P6" s="12" t="s">
         <v>29</v>
       </c>
       <c r="Q6" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="R6" s="36"/>
+      <c r="R6" s="26"/>
       <c r="S6" s="9" t="s">
         <v>35</v>
       </c>
       <c r="T6" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="U6" s="36"/>
+      <c r="U6" s="26"/>
       <c r="V6" s="8"/>
-      <c r="X6" s="23"/>
-      <c r="Y6" s="23"/>
-      <c r="Z6" s="23"/>
-      <c r="AA6" s="23"/>
-      <c r="AB6" s="23"/>
-      <c r="AC6" s="23"/>
+      <c r="X6" s="15"/>
+      <c r="Y6" s="15"/>
+      <c r="Z6" s="15"/>
+      <c r="AA6" s="15"/>
+      <c r="AB6" s="15"/>
+      <c r="AC6" s="15"/>
       <c r="AD6" s="8"/>
-      <c r="AF6" s="23"/>
-      <c r="AG6" s="23"/>
-      <c r="AH6" s="23"/>
-      <c r="AI6" s="23"/>
-      <c r="AJ6" s="23"/>
-      <c r="AK6" s="23"/>
-      <c r="AL6" s="23"/>
-      <c r="AM6" s="28"/>
-      <c r="AN6" s="28"/>
+      <c r="AF6" s="15"/>
+      <c r="AG6" s="15"/>
+      <c r="AH6" s="15"/>
+      <c r="AI6" s="15"/>
+      <c r="AJ6" s="15"/>
+      <c r="AK6" s="15"/>
+      <c r="AL6" s="15"/>
+      <c r="AM6" s="38"/>
+      <c r="AN6" s="38"/>
     </row>
     <row r="8" spans="2:42" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
@@ -11596,41 +11719,41 @@
       <c r="AO9" s="4"/>
     </row>
     <row r="10" spans="2:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13">
+      <c r="C10" s="25"/>
+      <c r="D10" s="25">
         <v>0</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="25">
         <v>2</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="25">
         <v>205</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="25">
         <v>214</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="25">
         <v>10</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="25">
         <v>8.51</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="25">
         <v>1.25</v>
       </c>
-      <c r="K10" s="13">
+      <c r="K10" s="25">
         <v>66</v>
       </c>
-      <c r="L10" s="13">
+      <c r="L10" s="25">
         <v>66</v>
       </c>
-      <c r="M10" s="13">
+      <c r="M10" s="25">
         <v>66</v>
       </c>
-      <c r="N10" s="13">
+      <c r="N10" s="25">
         <v>66</v>
       </c>
       <c r="O10" s="5" t="s">
@@ -11654,72 +11777,72 @@
       <c r="U10" s="2">
         <v>10</v>
       </c>
-      <c r="V10" s="15"/>
-      <c r="W10" s="14"/>
-      <c r="X10" s="13">
+      <c r="V10" s="33"/>
+      <c r="W10" s="34"/>
+      <c r="X10" s="25">
         <v>66</v>
       </c>
-      <c r="Y10" s="13">
+      <c r="Y10" s="25">
         <v>66</v>
       </c>
-      <c r="Z10" s="13">
+      <c r="Z10" s="25">
         <v>67</v>
       </c>
-      <c r="AA10" s="13">
+      <c r="AA10" s="25">
         <v>66</v>
       </c>
-      <c r="AB10" s="13">
+      <c r="AB10" s="25">
         <v>66</v>
       </c>
-      <c r="AC10" s="13">
+      <c r="AC10" s="25">
         <v>67</v>
       </c>
-      <c r="AD10" s="15"/>
-      <c r="AE10" s="14"/>
-      <c r="AF10" s="13">
+      <c r="AD10" s="33"/>
+      <c r="AE10" s="34"/>
+      <c r="AF10" s="25">
         <v>44</v>
       </c>
-      <c r="AG10" s="13">
+      <c r="AG10" s="25">
         <v>157</v>
       </c>
-      <c r="AH10" s="13">
+      <c r="AH10" s="25">
         <v>106</v>
       </c>
-      <c r="AI10" s="13">
+      <c r="AI10" s="25">
         <v>2</v>
       </c>
-      <c r="AJ10" s="13">
+      <c r="AJ10" s="25">
         <v>0</v>
       </c>
-      <c r="AK10" s="13">
+      <c r="AK10" s="25">
         <v>0</v>
       </c>
-      <c r="AL10" s="13">
+      <c r="AL10" s="25">
         <v>10</v>
       </c>
-      <c r="AM10" s="13">
+      <c r="AM10" s="25">
         <v>5.7450000000000001</v>
       </c>
-      <c r="AN10" s="13">
+      <c r="AN10" s="25">
         <v>6.3630000000000004</v>
       </c>
-      <c r="AO10" s="15"/>
-      <c r="AP10" s="17"/>
+      <c r="AO10" s="33"/>
+      <c r="AP10" s="39"/>
     </row>
     <row r="11" spans="2:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="16"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
       <c r="O11" s="5" t="s">
         <v>56</v>
       </c>
@@ -11741,64 +11864,64 @@
       <c r="U11" s="2">
         <v>11</v>
       </c>
-      <c r="V11" s="15"/>
-      <c r="W11" s="14"/>
-      <c r="X11" s="13"/>
-      <c r="Y11" s="13"/>
-      <c r="Z11" s="13"/>
-      <c r="AA11" s="13"/>
-      <c r="AB11" s="13"/>
-      <c r="AC11" s="13"/>
-      <c r="AD11" s="15"/>
-      <c r="AE11" s="14"/>
-      <c r="AF11" s="13"/>
-      <c r="AG11" s="13"/>
-      <c r="AH11" s="13"/>
-      <c r="AI11" s="13"/>
-      <c r="AJ11" s="13"/>
-      <c r="AK11" s="13"/>
-      <c r="AL11" s="13"/>
-      <c r="AM11" s="13"/>
-      <c r="AN11" s="13"/>
-      <c r="AO11" s="15"/>
-      <c r="AP11" s="17"/>
+      <c r="V11" s="33"/>
+      <c r="W11" s="34"/>
+      <c r="X11" s="25"/>
+      <c r="Y11" s="25"/>
+      <c r="Z11" s="25"/>
+      <c r="AA11" s="25"/>
+      <c r="AB11" s="25"/>
+      <c r="AC11" s="25"/>
+      <c r="AD11" s="33"/>
+      <c r="AE11" s="34"/>
+      <c r="AF11" s="25"/>
+      <c r="AG11" s="25"/>
+      <c r="AH11" s="25"/>
+      <c r="AI11" s="25"/>
+      <c r="AJ11" s="25"/>
+      <c r="AK11" s="25"/>
+      <c r="AL11" s="25"/>
+      <c r="AM11" s="25"/>
+      <c r="AN11" s="25"/>
+      <c r="AO11" s="33"/>
+      <c r="AP11" s="39"/>
     </row>
     <row r="12" spans="2:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13">
+      <c r="C12" s="25"/>
+      <c r="D12" s="25">
         <v>2</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="25">
         <v>2</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="25">
         <v>145</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="25">
         <v>236</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="25">
         <v>10</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="25">
         <v>8.51</v>
       </c>
-      <c r="J12" s="13">
+      <c r="J12" s="25">
         <v>1.25</v>
       </c>
-      <c r="K12" s="13">
+      <c r="K12" s="25">
         <v>56</v>
       </c>
-      <c r="L12" s="13">
+      <c r="L12" s="25">
         <v>56</v>
       </c>
-      <c r="M12" s="13">
+      <c r="M12" s="25">
         <v>56</v>
       </c>
-      <c r="N12" s="13">
+      <c r="N12" s="25">
         <v>56</v>
       </c>
       <c r="O12" s="5" t="s">
@@ -11822,72 +11945,72 @@
       <c r="U12" s="2">
         <v>5</v>
       </c>
-      <c r="V12" s="15"/>
-      <c r="W12" s="14"/>
-      <c r="X12" s="13">
+      <c r="V12" s="33"/>
+      <c r="W12" s="34"/>
+      <c r="X12" s="25">
         <v>56</v>
       </c>
-      <c r="Y12" s="13">
+      <c r="Y12" s="25">
         <v>56</v>
       </c>
-      <c r="Z12" s="13">
+      <c r="Z12" s="25">
         <v>57</v>
       </c>
-      <c r="AA12" s="13">
+      <c r="AA12" s="25">
         <v>56</v>
       </c>
-      <c r="AB12" s="13">
+      <c r="AB12" s="25">
         <v>56</v>
       </c>
-      <c r="AC12" s="13">
+      <c r="AC12" s="25">
         <v>57</v>
       </c>
-      <c r="AD12" s="15"/>
-      <c r="AE12" s="14"/>
-      <c r="AF12" s="13">
+      <c r="AD12" s="33"/>
+      <c r="AE12" s="34"/>
+      <c r="AF12" s="25">
         <v>31</v>
       </c>
-      <c r="AG12" s="13">
+      <c r="AG12" s="25">
         <v>97</v>
       </c>
-      <c r="AH12" s="13">
+      <c r="AH12" s="25">
         <v>72</v>
       </c>
-      <c r="AI12" s="13">
+      <c r="AI12" s="25">
         <v>2</v>
       </c>
-      <c r="AJ12" s="13">
+      <c r="AJ12" s="25">
         <v>2</v>
       </c>
-      <c r="AK12" s="13">
+      <c r="AK12" s="25">
         <v>0</v>
       </c>
-      <c r="AL12" s="13">
+      <c r="AL12" s="25">
         <v>10</v>
       </c>
-      <c r="AM12" s="13">
+      <c r="AM12" s="25">
         <v>5.7450000000000001</v>
       </c>
-      <c r="AN12" s="13">
+      <c r="AN12" s="25">
         <v>5.6920000000000002</v>
       </c>
-      <c r="AO12" s="15"/>
-      <c r="AP12" s="17"/>
+      <c r="AO12" s="33"/>
+      <c r="AP12" s="39"/>
     </row>
     <row r="13" spans="2:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="16"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
       <c r="O13" s="5" t="s">
         <v>56</v>
       </c>
@@ -11909,27 +12032,27 @@
       <c r="U13" s="2">
         <v>11</v>
       </c>
-      <c r="V13" s="15"/>
-      <c r="W13" s="14"/>
-      <c r="X13" s="13"/>
-      <c r="Y13" s="13"/>
-      <c r="Z13" s="13"/>
-      <c r="AA13" s="13"/>
-      <c r="AB13" s="13"/>
-      <c r="AC13" s="13"/>
-      <c r="AD13" s="15"/>
-      <c r="AE13" s="14"/>
-      <c r="AF13" s="13"/>
-      <c r="AG13" s="13"/>
-      <c r="AH13" s="13"/>
-      <c r="AI13" s="13"/>
-      <c r="AJ13" s="13"/>
-      <c r="AK13" s="13"/>
-      <c r="AL13" s="13"/>
-      <c r="AM13" s="13"/>
-      <c r="AN13" s="13"/>
-      <c r="AO13" s="15"/>
-      <c r="AP13" s="17"/>
+      <c r="V13" s="33"/>
+      <c r="W13" s="34"/>
+      <c r="X13" s="25"/>
+      <c r="Y13" s="25"/>
+      <c r="Z13" s="25"/>
+      <c r="AA13" s="25"/>
+      <c r="AB13" s="25"/>
+      <c r="AC13" s="25"/>
+      <c r="AD13" s="33"/>
+      <c r="AE13" s="34"/>
+      <c r="AF13" s="25"/>
+      <c r="AG13" s="25"/>
+      <c r="AH13" s="25"/>
+      <c r="AI13" s="25"/>
+      <c r="AJ13" s="25"/>
+      <c r="AK13" s="25"/>
+      <c r="AL13" s="25"/>
+      <c r="AM13" s="25"/>
+      <c r="AN13" s="25"/>
+      <c r="AO13" s="33"/>
+      <c r="AP13" s="39"/>
     </row>
     <row r="14" spans="2:42" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
@@ -12142,41 +12265,41 @@
       <c r="AO15" s="4"/>
     </row>
     <row r="16" spans="2:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13">
+      <c r="C16" s="25"/>
+      <c r="D16" s="25">
         <v>2</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="25">
         <v>2</v>
       </c>
-      <c r="F16" s="13">
+      <c r="F16" s="25">
         <v>221</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G16" s="25">
         <v>318</v>
       </c>
-      <c r="H16" s="13">
+      <c r="H16" s="25">
         <v>10</v>
       </c>
-      <c r="I16" s="13">
+      <c r="I16" s="25">
         <v>8.51</v>
       </c>
-      <c r="J16" s="13">
+      <c r="J16" s="25">
         <v>1.25</v>
       </c>
-      <c r="K16" s="13">
+      <c r="K16" s="25">
         <v>58</v>
       </c>
-      <c r="L16" s="13">
+      <c r="L16" s="25">
         <v>58</v>
       </c>
-      <c r="M16" s="13">
+      <c r="M16" s="25">
         <v>58</v>
       </c>
-      <c r="N16" s="13">
+      <c r="N16" s="25">
         <v>58</v>
       </c>
       <c r="O16" s="5" t="s">
@@ -12200,72 +12323,72 @@
       <c r="U16" s="2">
         <v>3</v>
       </c>
-      <c r="V16" s="15"/>
-      <c r="W16" s="14"/>
-      <c r="X16" s="13">
+      <c r="V16" s="33"/>
+      <c r="W16" s="34"/>
+      <c r="X16" s="25">
         <v>58</v>
       </c>
-      <c r="Y16" s="13">
+      <c r="Y16" s="25">
         <v>58</v>
       </c>
-      <c r="Z16" s="13">
+      <c r="Z16" s="25">
         <v>59</v>
       </c>
-      <c r="AA16" s="13">
+      <c r="AA16" s="25">
         <v>58</v>
       </c>
-      <c r="AB16" s="13">
+      <c r="AB16" s="25">
         <v>58</v>
       </c>
-      <c r="AC16" s="13">
+      <c r="AC16" s="25">
         <v>59</v>
       </c>
-      <c r="AD16" s="15"/>
-      <c r="AE16" s="14"/>
-      <c r="AF16" s="13">
+      <c r="AD16" s="33"/>
+      <c r="AE16" s="34"/>
+      <c r="AF16" s="25">
         <v>46</v>
       </c>
-      <c r="AG16" s="13">
+      <c r="AG16" s="25">
         <v>160</v>
       </c>
-      <c r="AH16" s="13">
+      <c r="AH16" s="25">
         <v>147</v>
       </c>
-      <c r="AI16" s="13">
+      <c r="AI16" s="25">
         <v>2</v>
       </c>
-      <c r="AJ16" s="13">
+      <c r="AJ16" s="25">
         <v>2</v>
       </c>
-      <c r="AK16" s="13">
+      <c r="AK16" s="25">
         <v>0</v>
       </c>
-      <c r="AL16" s="13">
+      <c r="AL16" s="25">
         <v>10</v>
       </c>
-      <c r="AM16" s="13">
+      <c r="AM16" s="25">
         <v>5.7450000000000001</v>
       </c>
-      <c r="AN16" s="13">
+      <c r="AN16" s="25">
         <v>5.6920000000000002</v>
       </c>
-      <c r="AO16" s="15"/>
-      <c r="AP16" s="17"/>
+      <c r="AO16" s="33"/>
+      <c r="AP16" s="39"/>
     </row>
     <row r="17" spans="2:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="16"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
+      <c r="N17" s="25"/>
       <c r="O17" s="5" t="s">
         <v>56</v>
       </c>
@@ -12287,27 +12410,27 @@
       <c r="U17" s="2">
         <v>11</v>
       </c>
-      <c r="V17" s="15"/>
-      <c r="W17" s="14"/>
-      <c r="X17" s="13"/>
-      <c r="Y17" s="13"/>
-      <c r="Z17" s="13"/>
-      <c r="AA17" s="13"/>
-      <c r="AB17" s="13"/>
-      <c r="AC17" s="13"/>
-      <c r="AD17" s="15"/>
-      <c r="AE17" s="14"/>
-      <c r="AF17" s="13"/>
-      <c r="AG17" s="13"/>
-      <c r="AH17" s="13"/>
-      <c r="AI17" s="13"/>
-      <c r="AJ17" s="13"/>
-      <c r="AK17" s="13"/>
-      <c r="AL17" s="13"/>
-      <c r="AM17" s="13"/>
-      <c r="AN17" s="13"/>
-      <c r="AO17" s="15"/>
-      <c r="AP17" s="17"/>
+      <c r="V17" s="33"/>
+      <c r="W17" s="34"/>
+      <c r="X17" s="25"/>
+      <c r="Y17" s="25"/>
+      <c r="Z17" s="25"/>
+      <c r="AA17" s="25"/>
+      <c r="AB17" s="25"/>
+      <c r="AC17" s="25"/>
+      <c r="AD17" s="33"/>
+      <c r="AE17" s="34"/>
+      <c r="AF17" s="25"/>
+      <c r="AG17" s="25"/>
+      <c r="AH17" s="25"/>
+      <c r="AI17" s="25"/>
+      <c r="AJ17" s="25"/>
+      <c r="AK17" s="25"/>
+      <c r="AL17" s="25"/>
+      <c r="AM17" s="25"/>
+      <c r="AN17" s="25"/>
+      <c r="AO17" s="33"/>
+      <c r="AP17" s="39"/>
     </row>
     <row r="18" spans="2:42" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
@@ -13359,95 +13482,98 @@
       </c>
       <c r="AO27" s="4"/>
     </row>
-    <row r="28" spans="2:42" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="3" t="s">
-        <v>16</v>
-      </c>
+    <row r="28" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="4"/>
       <c r="D28" s="4">
         <v>0</v>
       </c>
-      <c r="E28" s="2">
-        <v>14</v>
-      </c>
-      <c r="F28" s="1">
-        <v>767</v>
-      </c>
-      <c r="G28" s="2">
-        <v>583</v>
-      </c>
-      <c r="H28" s="1">
+      <c r="E28" s="4">
+        <v>2</v>
+      </c>
+      <c r="F28" s="4">
+        <v>81</v>
+      </c>
+      <c r="G28" s="4">
+        <v>107</v>
+      </c>
+      <c r="H28" s="4">
         <v>10</v>
       </c>
-      <c r="I28" s="2">
-        <v>8.7420000000000009</v>
-      </c>
-      <c r="J28" s="5">
+      <c r="I28" s="4">
+        <v>6.38</v>
+      </c>
+      <c r="J28" s="4">
         <v>1.25</v>
       </c>
-      <c r="K28" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="L28" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="M28" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="N28" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="O28" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="P28" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q28" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="R28" s="2">
-        <v>4</v>
-      </c>
-      <c r="S28" s="5">
-        <v>1</v>
-      </c>
-      <c r="T28" s="2">
-        <v>1</v>
-      </c>
-      <c r="U28" s="2" t="s">
-        <v>45</v>
-      </c>
+      <c r="K28" s="4">
+        <v>31</v>
+      </c>
+      <c r="L28" s="4">
+        <v>31</v>
+      </c>
+      <c r="M28" s="4">
+        <v>31</v>
+      </c>
+      <c r="N28" s="4">
+        <v>31</v>
+      </c>
+      <c r="O28" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="P28" s="4">
+        <v>30</v>
+      </c>
+      <c r="Q28" s="4">
+        <v>30</v>
+      </c>
+      <c r="R28" s="4">
+        <v>3</v>
+      </c>
+      <c r="S28" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="T28" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="U28" s="4">
+        <v>10</v>
+      </c>
+      <c r="V28" s="4"/>
       <c r="X28" s="4">
-        <v>13</v>
-      </c>
-      <c r="Y28" s="2">
-        <v>13</v>
-      </c>
-      <c r="Z28" s="1">
-        <v>13</v>
-      </c>
-      <c r="AA28" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB28" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC28" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF28" s="4">
-        <v>231</v>
+        <v>31</v>
+      </c>
+      <c r="Y28" s="4">
+        <v>31</v>
+      </c>
+      <c r="Z28" s="4">
+        <v>32</v>
+      </c>
+      <c r="AA28" s="4">
+        <v>31</v>
+      </c>
+      <c r="AB28" s="4">
+        <v>31</v>
+      </c>
+      <c r="AC28" s="4">
+        <v>32</v>
+      </c>
+      <c r="AD28" s="4"/>
+      <c r="AF28" s="2">
+        <v>15</v>
       </c>
       <c r="AG28" s="2">
-        <v>739</v>
-      </c>
-      <c r="AH28" s="1">
-        <v>699</v>
-      </c>
-      <c r="AI28" s="2">
-        <v>0</v>
-      </c>
-      <c r="AJ28" s="1">
+        <v>50</v>
+      </c>
+      <c r="AH28" s="2">
+        <v>24</v>
+      </c>
+      <c r="AI28" s="4">
+        <v>2</v>
+      </c>
+      <c r="AJ28" s="2">
         <v>0</v>
       </c>
       <c r="AK28" s="4">
@@ -13457,50 +13583,205 @@
         <v>10</v>
       </c>
       <c r="AM28" s="4">
+        <v>5.4290000000000003</v>
+      </c>
+      <c r="AN28" s="2">
+        <v>5.6920000000000002</v>
+      </c>
+      <c r="AO28" s="4"/>
+    </row>
+    <row r="29" spans="2:42" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="4">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2">
+        <v>14</v>
+      </c>
+      <c r="F29" s="1">
+        <v>767</v>
+      </c>
+      <c r="G29" s="2">
+        <v>583</v>
+      </c>
+      <c r="H29" s="1">
+        <v>10</v>
+      </c>
+      <c r="I29" s="2">
+        <v>8.7420000000000009</v>
+      </c>
+      <c r="J29" s="5">
+        <v>1.25</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N29" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="O29" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="P29" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q29" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="R29" s="2">
+        <v>4</v>
+      </c>
+      <c r="S29" s="5">
+        <v>1</v>
+      </c>
+      <c r="T29" s="2">
+        <v>1</v>
+      </c>
+      <c r="U29" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="V29" s="4"/>
+      <c r="X29" s="4">
+        <v>13</v>
+      </c>
+      <c r="Y29" s="2">
+        <v>13</v>
+      </c>
+      <c r="Z29" s="1">
+        <v>13</v>
+      </c>
+      <c r="AA29" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB29" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC29" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD29" s="4"/>
+      <c r="AF29" s="4">
+        <v>231</v>
+      </c>
+      <c r="AG29" s="2">
+        <v>739</v>
+      </c>
+      <c r="AH29" s="1">
+        <v>699</v>
+      </c>
+      <c r="AI29" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ29" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK29" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL29" s="4">
+        <v>10</v>
+      </c>
+      <c r="AM29" s="4">
         <v>7.2690000000000001</v>
       </c>
-      <c r="AN28" s="4">
+      <c r="AN29" s="4">
         <v>8.202</v>
       </c>
-      <c r="AO28" s="4"/>
+      <c r="AO29" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="142">
-    <mergeCell ref="X4:X6"/>
-    <mergeCell ref="Y4:Y6"/>
-    <mergeCell ref="Z4:Z6"/>
-    <mergeCell ref="AA4:AA6"/>
-    <mergeCell ref="AB4:AB6"/>
-    <mergeCell ref="AC4:AC6"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="I4:I6"/>
-    <mergeCell ref="J4:J6"/>
-    <mergeCell ref="K4:L5"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="U5:U6"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="K3:U3"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="O4:U4"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="M4:N5"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="X16:X17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="AC16:AC17"/>
+    <mergeCell ref="AB16:AB17"/>
+    <mergeCell ref="AA16:AA17"/>
+    <mergeCell ref="Z16:Z17"/>
+    <mergeCell ref="Y16:Y17"/>
+    <mergeCell ref="AH16:AH17"/>
+    <mergeCell ref="AG16:AG17"/>
+    <mergeCell ref="AF16:AF17"/>
+    <mergeCell ref="AE16:AE17"/>
+    <mergeCell ref="AD16:AD17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="V16:V17"/>
+    <mergeCell ref="W16:W17"/>
+    <mergeCell ref="AP10:AP11"/>
+    <mergeCell ref="AO10:AO11"/>
+    <mergeCell ref="AP12:AP13"/>
+    <mergeCell ref="AO12:AO13"/>
+    <mergeCell ref="AP16:AP17"/>
+    <mergeCell ref="AO16:AO17"/>
+    <mergeCell ref="AN16:AN17"/>
+    <mergeCell ref="AM16:AM17"/>
+    <mergeCell ref="AL16:AL17"/>
+    <mergeCell ref="AK16:AK17"/>
+    <mergeCell ref="AJ16:AJ17"/>
+    <mergeCell ref="AI16:AI17"/>
+    <mergeCell ref="AD10:AD11"/>
+    <mergeCell ref="AE10:AE11"/>
+    <mergeCell ref="AD12:AD13"/>
+    <mergeCell ref="AE12:AE13"/>
+    <mergeCell ref="AI12:AI13"/>
+    <mergeCell ref="AJ12:AJ13"/>
+    <mergeCell ref="AK12:AK13"/>
+    <mergeCell ref="AL12:AL13"/>
+    <mergeCell ref="AN12:AN13"/>
+    <mergeCell ref="AM12:AM13"/>
+    <mergeCell ref="AC12:AC13"/>
+    <mergeCell ref="AF12:AF13"/>
+    <mergeCell ref="AG12:AG13"/>
+    <mergeCell ref="AH12:AH13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="Y12:Y13"/>
+    <mergeCell ref="Z12:Z13"/>
+    <mergeCell ref="AA12:AA13"/>
+    <mergeCell ref="AB12:AB13"/>
+    <mergeCell ref="W12:W13"/>
+    <mergeCell ref="V12:V13"/>
+    <mergeCell ref="AM10:AM11"/>
+    <mergeCell ref="AN10:AN11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="X12:X13"/>
+    <mergeCell ref="AH10:AH11"/>
+    <mergeCell ref="AI10:AI11"/>
+    <mergeCell ref="AJ10:AJ11"/>
+    <mergeCell ref="AK10:AK11"/>
+    <mergeCell ref="AL10:AL11"/>
+    <mergeCell ref="AA10:AA11"/>
+    <mergeCell ref="AB10:AB11"/>
+    <mergeCell ref="AC10:AC11"/>
+    <mergeCell ref="AF10:AF11"/>
     <mergeCell ref="AG10:AG11"/>
     <mergeCell ref="M10:M11"/>
     <mergeCell ref="N10:N11"/>
@@ -13525,89 +13806,41 @@
     <mergeCell ref="AA3:AC3"/>
     <mergeCell ref="X2:AC2"/>
     <mergeCell ref="D2:U2"/>
-    <mergeCell ref="AM10:AM11"/>
-    <mergeCell ref="AN10:AN11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="X12:X13"/>
-    <mergeCell ref="AH10:AH11"/>
-    <mergeCell ref="AI10:AI11"/>
-    <mergeCell ref="AJ10:AJ11"/>
-    <mergeCell ref="AK10:AK11"/>
-    <mergeCell ref="AL10:AL11"/>
-    <mergeCell ref="AA10:AA11"/>
-    <mergeCell ref="AB10:AB11"/>
-    <mergeCell ref="AC10:AC11"/>
-    <mergeCell ref="AF10:AF11"/>
-    <mergeCell ref="AN12:AN13"/>
-    <mergeCell ref="AM12:AM13"/>
-    <mergeCell ref="AC12:AC13"/>
-    <mergeCell ref="AF12:AF13"/>
-    <mergeCell ref="AG12:AG13"/>
-    <mergeCell ref="AH12:AH13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="Y12:Y13"/>
-    <mergeCell ref="Z12:Z13"/>
-    <mergeCell ref="AA12:AA13"/>
-    <mergeCell ref="AB12:AB13"/>
-    <mergeCell ref="W12:W13"/>
-    <mergeCell ref="V12:V13"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="V16:V17"/>
-    <mergeCell ref="W16:W17"/>
-    <mergeCell ref="AP10:AP11"/>
-    <mergeCell ref="AO10:AO11"/>
-    <mergeCell ref="AP12:AP13"/>
-    <mergeCell ref="AO12:AO13"/>
-    <mergeCell ref="AP16:AP17"/>
-    <mergeCell ref="AO16:AO17"/>
-    <mergeCell ref="AN16:AN17"/>
-    <mergeCell ref="AM16:AM17"/>
-    <mergeCell ref="AL16:AL17"/>
-    <mergeCell ref="AK16:AK17"/>
-    <mergeCell ref="AJ16:AJ17"/>
-    <mergeCell ref="AI16:AI17"/>
-    <mergeCell ref="AD10:AD11"/>
-    <mergeCell ref="AE10:AE11"/>
-    <mergeCell ref="AD12:AD13"/>
-    <mergeCell ref="AE12:AE13"/>
-    <mergeCell ref="AI12:AI13"/>
-    <mergeCell ref="AJ12:AJ13"/>
-    <mergeCell ref="AK12:AK13"/>
-    <mergeCell ref="AL12:AL13"/>
-    <mergeCell ref="AC16:AC17"/>
-    <mergeCell ref="AB16:AB17"/>
-    <mergeCell ref="AA16:AA17"/>
-    <mergeCell ref="Z16:Z17"/>
-    <mergeCell ref="Y16:Y17"/>
-    <mergeCell ref="AH16:AH17"/>
-    <mergeCell ref="AG16:AG17"/>
-    <mergeCell ref="AF16:AF17"/>
-    <mergeCell ref="AE16:AE17"/>
-    <mergeCell ref="AD16:AD17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="X16:X17"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="O4:U4"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="M4:N5"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="U5:U6"/>
+    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="K3:U3"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="X4:X6"/>
+    <mergeCell ref="Y4:Y6"/>
+    <mergeCell ref="Z4:Z6"/>
+    <mergeCell ref="AA4:AA6"/>
+    <mergeCell ref="AB4:AB6"/>
+    <mergeCell ref="AC4:AC6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="I4:I6"/>
+    <mergeCell ref="J4:J6"/>
+    <mergeCell ref="K4:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -13619,7 +13852,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AH18" sqref="AH18"/>
+      <selection activeCell="AH16" sqref="AH16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13633,7 +13866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{543676F3-4F14-4D41-B3B3-EE3B633252FE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>

</xml_diff>